<commit_message>
Add chesterfield occupations and update 1b-4
developed script to compute ability to pay
</commit_message>
<xml_diff>
--- a/data/costar_rent_avg.xlsx
+++ b/data/costar_rent_avg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\chesterfield-market-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7389954F-C1F5-4F34-B299-DB6FD3659A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76A990B-EE9C-4F64-8BE3-1C7B54B12013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9984" yWindow="744" windowWidth="9396" windowHeight="9504" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Market Asking Rent Per Unit" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>2022 YTD</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>2021</t>
   </si>
@@ -55,9 +52,6 @@
     <t>2012</t>
   </si>
   <si>
-    <t>2011</t>
-  </si>
-  <si>
     <t>2010</t>
   </si>
   <si>
@@ -91,19 +85,16 @@
     <t>2000</t>
   </si>
   <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>marketrent</t>
+    <t>askingrent</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="\$##,###,###,##0_);[Red]\(\$##,###,###,##0\)"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -165,14 +156,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -480,10 +471,10 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -494,23 +485,23 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>0</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1444</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
       </c>
       <c r="B3" s="7">
         <v>1420</v>
@@ -518,15 +509,15 @@
     </row>
     <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>2</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1359</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>3</v>
       </c>
       <c r="B5" s="7">
         <v>1290</v>
@@ -534,15 +525,15 @@
     </row>
     <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="B6" s="4">
-        <v>1277</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>5</v>
       </c>
       <c r="B7" s="7">
         <v>1257</v>
@@ -550,15 +541,15 @@
     </row>
     <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="B8" s="4">
-        <v>1233</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>7</v>
       </c>
       <c r="B9" s="7">
         <v>1221</v>
@@ -566,15 +557,15 @@
     </row>
     <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="B10" s="4">
-        <v>1184</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="B11" s="7">
         <v>1171</v>
@@ -582,15 +573,15 @@
     </row>
     <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="4">
+        <v>9</v>
+      </c>
+      <c r="B12" s="6">
         <v>1150</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>11</v>
+    <row r="13" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>2011</v>
       </c>
       <c r="B13" s="7">
         <v>1156</v>
@@ -598,15 +589,15 @@
     </row>
     <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="4">
+        <v>10</v>
+      </c>
+      <c r="B14" s="6">
         <v>1193</v>
       </c>
     </row>
-    <row r="15" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>13</v>
+    <row r="15" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="B15" s="7">
         <v>1224</v>
@@ -614,15 +605,15 @@
     </row>
     <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="4">
+        <v>12</v>
+      </c>
+      <c r="B16" s="6">
         <v>1251</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>15</v>
+    <row r="17" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="B17" s="7">
         <v>1272</v>
@@ -630,15 +621,15 @@
     </row>
     <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="4">
+        <v>14</v>
+      </c>
+      <c r="B18" s="6">
         <v>1298</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>17</v>
+    <row r="19" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="B19" s="7">
         <v>1270</v>
@@ -646,15 +637,15 @@
     </row>
     <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="4">
+        <v>16</v>
+      </c>
+      <c r="B20" s="6">
         <v>1293</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>19</v>
+    <row r="21" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="B21" s="7">
         <v>1319</v>
@@ -662,15 +653,15 @@
     </row>
     <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="4">
+        <v>18</v>
+      </c>
+      <c r="B22" s="6">
         <v>1376</v>
       </c>
     </row>
-    <row r="23" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
-        <v>21</v>
+    <row r="23" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="B23" s="7">
         <v>1414</v>
@@ -678,9 +669,9 @@
     </row>
     <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="4">
+        <v>20</v>
+      </c>
+      <c r="B24" s="6">
         <v>1331</v>
       </c>
     </row>

</xml_diff>